<commit_message>
update input excel, add price infomation for Years 2041-2050
</commit_message>
<xml_diff>
--- a/InputDataCoalUpdated.xlsx
+++ b/InputDataCoalUpdated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simoneosei/Documents/GitHub/ffrm_python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zl17868/Documents/ffrm_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF039AAE-6848-B04A-8233-4B8750451D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E2C87C-5172-A84A-B47A-C56B4E47C02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CoalPlantData" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="101">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -916,12 +916,12 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A15"/>
+      <selection activeCell="A16" sqref="A16:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.83203125" customWidth="1"/>
+    <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="5" width="13.83203125" customWidth="1"/>
@@ -1260,9 +1260,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="A16" s="3"/>
       <c r="B16" s="6" t="s">
         <v>0</v>
       </c>
@@ -1283,9 +1281,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="A17" s="3"/>
       <c r="B17" s="6" t="s">
         <v>0</v>
       </c>
@@ -1306,9 +1302,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="A18" s="3"/>
       <c r="B18" s="6" t="s">
         <v>0</v>
       </c>
@@ -1329,9 +1323,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="A19" s="3"/>
       <c r="B19" s="6" t="s">
         <v>0</v>
       </c>
@@ -3787,13 +3779,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.5" customWidth="1"/>
+    <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="31" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13249,7 +13241,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:K33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13341,7 +13335,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="21">
-        <f t="shared" ref="A5:A23" si="0">A4+1</f>
+        <f t="shared" ref="A5:A33" si="0">A4+1</f>
         <v>2022</v>
       </c>
       <c r="B5" s="11">
@@ -14082,31 +14076,381 @@
         <v>0.67466069000507511</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="21">
+        <f t="shared" si="0"/>
+        <v>2041</v>
+      </c>
+      <c r="B24" s="11">
+        <v>2.1908344190476199</v>
+      </c>
+      <c r="C24" s="11">
+        <v>1.61642955640051</v>
+      </c>
+      <c r="D24" s="11">
+        <v>1.3984974952381</v>
+      </c>
+      <c r="E24" s="11">
+        <v>1.28052865296804</v>
+      </c>
+      <c r="F24" s="11">
+        <v>1.1954705631659099</v>
+      </c>
+      <c r="G24" s="11">
+        <v>1.1345047716895</v>
+      </c>
+      <c r="H24" s="11">
+        <v>1.01229800196367</v>
+      </c>
+      <c r="I24" s="11">
+        <v>0.90847234906138896</v>
+      </c>
+      <c r="J24" s="11">
+        <v>0.82517252409944197</v>
+      </c>
+      <c r="K24" s="11">
+        <v>0.674660690005075</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="21">
+        <f t="shared" si="0"/>
+        <v>2042</v>
+      </c>
+      <c r="B25" s="11">
+        <v>2.1908344190476199</v>
+      </c>
+      <c r="C25" s="11">
+        <v>1.61642955640051</v>
+      </c>
+      <c r="D25" s="11">
+        <v>1.3984974952381</v>
+      </c>
+      <c r="E25" s="11">
+        <v>1.28052865296804</v>
+      </c>
+      <c r="F25" s="11">
+        <v>1.1954705631659099</v>
+      </c>
+      <c r="G25" s="11">
+        <v>1.1345047716895</v>
+      </c>
+      <c r="H25" s="11">
+        <v>1.01229800196367</v>
+      </c>
+      <c r="I25" s="11">
+        <v>0.90847234906138896</v>
+      </c>
+      <c r="J25" s="11">
+        <v>0.82517252409944197</v>
+      </c>
+      <c r="K25" s="11">
+        <v>0.674660690005075</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="21">
+        <f t="shared" si="0"/>
+        <v>2043</v>
+      </c>
+      <c r="B26" s="11">
+        <v>2.1908344190476199</v>
+      </c>
+      <c r="C26" s="11">
+        <v>1.61642955640051</v>
+      </c>
+      <c r="D26" s="11">
+        <v>1.3984974952381</v>
+      </c>
+      <c r="E26" s="11">
+        <v>1.28052865296804</v>
+      </c>
+      <c r="F26" s="11">
+        <v>1.1954705631659099</v>
+      </c>
+      <c r="G26" s="11">
+        <v>1.1345047716895</v>
+      </c>
+      <c r="H26" s="11">
+        <v>1.01229800196367</v>
+      </c>
+      <c r="I26" s="11">
+        <v>0.90847234906138896</v>
+      </c>
+      <c r="J26" s="11">
+        <v>0.82517252409944197</v>
+      </c>
+      <c r="K26" s="11">
+        <v>0.674660690005075</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="21">
+        <f t="shared" si="0"/>
+        <v>2044</v>
+      </c>
+      <c r="B27" s="11">
+        <v>2.1908344190476199</v>
+      </c>
+      <c r="C27" s="11">
+        <v>1.61642955640051</v>
+      </c>
+      <c r="D27" s="11">
+        <v>1.3984974952381</v>
+      </c>
+      <c r="E27" s="11">
+        <v>1.28052865296804</v>
+      </c>
+      <c r="F27" s="11">
+        <v>1.1954705631659099</v>
+      </c>
+      <c r="G27" s="11">
+        <v>1.1345047716895</v>
+      </c>
+      <c r="H27" s="11">
+        <v>1.01229800196367</v>
+      </c>
+      <c r="I27" s="11">
+        <v>0.90847234906138896</v>
+      </c>
+      <c r="J27" s="11">
+        <v>0.82517252409944197</v>
+      </c>
+      <c r="K27" s="11">
+        <v>0.674660690005075</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="21">
+        <f t="shared" si="0"/>
+        <v>2045</v>
+      </c>
+      <c r="B28" s="11">
+        <v>2.1908344190476199</v>
+      </c>
+      <c r="C28" s="11">
+        <v>1.61642955640051</v>
+      </c>
+      <c r="D28" s="11">
+        <v>1.3984974952381</v>
+      </c>
+      <c r="E28" s="11">
+        <v>1.28052865296804</v>
+      </c>
+      <c r="F28" s="11">
+        <v>1.1954705631659099</v>
+      </c>
+      <c r="G28" s="11">
+        <v>1.1345047716895</v>
+      </c>
+      <c r="H28" s="11">
+        <v>1.01229800196367</v>
+      </c>
+      <c r="I28" s="11">
+        <v>0.90847234906138896</v>
+      </c>
+      <c r="J28" s="11">
+        <v>0.82517252409944197</v>
+      </c>
+      <c r="K28" s="11">
+        <v>0.674660690005075</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="21">
+        <f t="shared" si="0"/>
+        <v>2046</v>
+      </c>
+      <c r="B29" s="11">
+        <v>2.1908344190476199</v>
+      </c>
+      <c r="C29" s="11">
+        <v>1.61642955640051</v>
+      </c>
+      <c r="D29" s="11">
+        <v>1.3984974952381</v>
+      </c>
+      <c r="E29" s="11">
+        <v>1.28052865296804</v>
+      </c>
+      <c r="F29" s="11">
+        <v>1.1954705631659099</v>
+      </c>
+      <c r="G29" s="11">
+        <v>1.1345047716895</v>
+      </c>
+      <c r="H29" s="11">
+        <v>1.01229800196367</v>
+      </c>
+      <c r="I29" s="11">
+        <v>0.90847234906138896</v>
+      </c>
+      <c r="J29" s="11">
+        <v>0.82517252409944197</v>
+      </c>
+      <c r="K29" s="11">
+        <v>0.674660690005075</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="21">
+        <f t="shared" si="0"/>
+        <v>2047</v>
+      </c>
+      <c r="B30" s="11">
+        <v>2.1908344190476199</v>
+      </c>
+      <c r="C30" s="11">
+        <v>1.61642955640051</v>
+      </c>
+      <c r="D30" s="11">
+        <v>1.3984974952381</v>
+      </c>
+      <c r="E30" s="11">
+        <v>1.28052865296804</v>
+      </c>
+      <c r="F30" s="11">
+        <v>1.1954705631659099</v>
+      </c>
+      <c r="G30" s="11">
+        <v>1.1345047716895</v>
+      </c>
+      <c r="H30" s="11">
+        <v>1.01229800196367</v>
+      </c>
+      <c r="I30" s="11">
+        <v>0.90847234906138896</v>
+      </c>
+      <c r="J30" s="11">
+        <v>0.82517252409944197</v>
+      </c>
+      <c r="K30" s="11">
+        <v>0.674660690005075</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="21">
+        <f t="shared" si="0"/>
+        <v>2048</v>
+      </c>
+      <c r="B31" s="11">
+        <v>2.1908344190476199</v>
+      </c>
+      <c r="C31" s="11">
+        <v>1.61642955640051</v>
+      </c>
+      <c r="D31" s="11">
+        <v>1.3984974952381</v>
+      </c>
+      <c r="E31" s="11">
+        <v>1.28052865296804</v>
+      </c>
+      <c r="F31" s="11">
+        <v>1.1954705631659099</v>
+      </c>
+      <c r="G31" s="11">
+        <v>1.1345047716895</v>
+      </c>
+      <c r="H31" s="11">
+        <v>1.01229800196367</v>
+      </c>
+      <c r="I31" s="11">
+        <v>0.90847234906138896</v>
+      </c>
+      <c r="J31" s="11">
+        <v>0.82517252409944197</v>
+      </c>
+      <c r="K31" s="11">
+        <v>0.674660690005075</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="21">
+        <f t="shared" si="0"/>
+        <v>2049</v>
+      </c>
+      <c r="B32" s="11">
+        <v>2.1908344190476199</v>
+      </c>
+      <c r="C32" s="11">
+        <v>1.61642955640051</v>
+      </c>
+      <c r="D32" s="11">
+        <v>1.3984974952381</v>
+      </c>
+      <c r="E32" s="11">
+        <v>1.28052865296804</v>
+      </c>
+      <c r="F32" s="11">
+        <v>1.1954705631659099</v>
+      </c>
+      <c r="G32" s="11">
+        <v>1.1345047716895</v>
+      </c>
+      <c r="H32" s="11">
+        <v>1.01229800196367</v>
+      </c>
+      <c r="I32" s="11">
+        <v>0.90847234906138896</v>
+      </c>
+      <c r="J32" s="11">
+        <v>0.82517252409944197</v>
+      </c>
+      <c r="K32" s="11">
+        <v>0.674660690005075</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="21">
+        <f t="shared" si="0"/>
+        <v>2050</v>
+      </c>
+      <c r="B33" s="11">
+        <v>2.1908344190476199</v>
+      </c>
+      <c r="C33" s="11">
+        <v>1.61642955640051</v>
+      </c>
+      <c r="D33" s="11">
+        <v>1.3984974952381</v>
+      </c>
+      <c r="E33" s="11">
+        <v>1.28052865296804</v>
+      </c>
+      <c r="F33" s="11">
+        <v>1.1954705631659099</v>
+      </c>
+      <c r="G33" s="11">
+        <v>1.1345047716895</v>
+      </c>
+      <c r="H33" s="11">
+        <v>1.01229800196367</v>
+      </c>
+      <c r="I33" s="11">
+        <v>0.90847234906138896</v>
+      </c>
+      <c r="J33" s="11">
+        <v>0.82517252409944197</v>
+      </c>
+      <c r="K33" s="11">
+        <v>0.674660690005075</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Incorporating log infeasibility constraint function
</commit_message>
<xml_diff>
--- a/InputDataCoalUpdated.xlsx
+++ b/InputDataCoalUpdated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zl17868/Documents/ffrm_python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simoneosei/Documents/GitHub/ffrm_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E2C87C-5172-A84A-B47A-C56B4E47C02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88235084-5EE6-8340-ADBD-ECF37550280F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16260" windowHeight="17500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CoalPlantData" sheetId="1" r:id="rId1"/>
@@ -3779,8 +3779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A17"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13241,8 +13241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:K33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15413,7 +15413,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:C1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15493,7 +15495,7 @@
         <v>63</v>
       </c>
       <c r="B9" s="32">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>64</v>
@@ -15515,7 +15517,7 @@
         <v>67</v>
       </c>
       <c r="B11" s="35">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>68</v>

</xml_diff>